<commit_message>
Update English resource with full sentences
</commit_message>
<xml_diff>
--- a/assets/files/samples/english_pattern.xlsx
+++ b/assets/files/samples/english_pattern.xlsx
@@ -412,226 +412,226 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>I'm gonna...</v>
+        <v>I'm gonna grab some coffee.</v>
       </c>
       <c r="B2" t="str">
-        <v>나 ~할 거야. (계획/의지)</v>
+        <v>나 커피 좀 사러 갈 거야.</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>I didn't mean to...</v>
+        <v>I didn't mean to hurt your feelings.</v>
       </c>
       <c r="B3" t="str">
-        <v>~하려던 게 아니었어. (실수/사과)</v>
+        <v>네 기분을 상하게 하려던 건 아니었어.</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Are you sure you want to...?</v>
+        <v>Are you sure you want to quit?</v>
       </c>
       <c r="B4" t="str">
-        <v>정말 ~하고 싶은 거 맞아?</v>
+        <v>정말 그만두고 싶은 거 맞아?</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
-        <v>I'm here to...</v>
+        <v>I'm here to see Mr. Kim.</v>
       </c>
       <c r="B5" t="str">
-        <v>~하러 왔어. (목적)</v>
+        <v>김 선생님을 뵈러 왔습니다.</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
-        <v>It looks like...</v>
+        <v>It looks like it's going to rain.</v>
       </c>
       <c r="B6" t="str">
-        <v>~인 것 같아. (추측)</v>
+        <v>비가 올 것 같아.</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
-        <v>How about...?</v>
+        <v>How about we go out for dinner?</v>
       </c>
       <c r="B7" t="str">
-        <v>~하는 게 어때? (제안)</v>
+        <v>우리 저녁 먹으러 나가는 거 어때?</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
-        <v>Why don't you...?</v>
+        <v>Why don't you take a break?</v>
       </c>
       <c r="B8" t="str">
-        <v>~하는 게 어때? (권유)</v>
+        <v>좀 쉬는 게 어때?</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
-        <v>I used to...</v>
+        <v>I used to play the piano.</v>
       </c>
       <c r="B9" t="str">
-        <v>예전엔 ~하곤 했어. (과거 습관)</v>
+        <v>예전엔 피아노를 치곤 했어.</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="str">
-        <v>I'd like to...</v>
+        <v>I'd like to make a reservation.</v>
       </c>
       <c r="B10" t="str">
-        <v>~하고 싶은 기분이야. (정중한 희망)</v>
+        <v>예약을 하고 싶은데요.</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
-        <v>Do you mind if I...?</v>
+        <v>Do you mind if I sit here?</v>
       </c>
       <c r="B11" t="str">
-        <v>내가 ~해도 될까? (허락)</v>
+        <v>여기 앉아도 될까요?</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
-        <v>What if...?</v>
+        <v>What if I fail the test?</v>
       </c>
       <c r="B12" t="str">
-        <v>만약 ~라면 어떡해? (가정)</v>
+        <v>시험에 떨어지면 어떡해?</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
-        <v>It's time to...</v>
+        <v>It's time to say goodbye.</v>
       </c>
       <c r="B13" t="str">
-        <v>~할 시간이야.</v>
+        <v>이제 헤어질 시간이야.</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>There is no need to...</v>
+        <v>There is no need to worry.</v>
       </c>
       <c r="B14" t="str">
-        <v>~할 필요 없어.</v>
+        <v>걱정할 필요 없어.</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
-        <v>Make sure to...</v>
+        <v>Make sure to lock the door.</v>
       </c>
       <c r="B15" t="str">
-        <v>꼭 ~하도록 해. (당부)</v>
+        <v>문 꼭 잠그도록 해.</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
-        <v>I'm looking forward to...</v>
+        <v>I'm looking forward to the party.</v>
       </c>
       <c r="B16" t="str">
-        <v>~을 기대하고 있어.</v>
+        <v>파티가 정말 기대돼.</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
-        <v>Can I get...?</v>
+        <v>Can I get a glass of water?</v>
       </c>
       <c r="B17" t="str">
-        <v>~좀 주시겠어요? (주문/요청)</v>
+        <v>물 한 잔 주시겠어요?</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>It takes [time] to...</v>
+        <v>It takes about an hour to get there.</v>
       </c>
       <c r="B18" t="str">
-        <v>~하는 데 [시간]이 걸려.</v>
+        <v>거기까지 가는 데 한 시간 정도 걸려.</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
-        <v>That's why...</v>
+        <v>That's why I was late.</v>
       </c>
       <c r="B19" t="str">
-        <v>그래서 ~한 거야. (이유)</v>
+        <v>그래서 늦은 거야.</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="str">
-        <v>I have no idea...</v>
+        <v>I have no idea what you're talking about.</v>
       </c>
       <c r="B20" t="str">
-        <v>~을 전혀 모르겠어.</v>
+        <v>무슨 말을 하는지 전혀 모르겠어.</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
-        <v>Let me...</v>
+        <v>Let me check my schedule.</v>
       </c>
       <c r="B21" t="str">
-        <v>내가 ~할게/하게 해줘.</v>
+        <v>내 일정 좀 확인해볼게.</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
-        <v>I feel like...</v>
+        <v>I feel like having pizza today.</v>
       </c>
       <c r="B22" t="str">
-        <v>~하고 싶은 기분이야.</v>
+        <v>오늘 피자 먹고 싶은 기분이야.</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
-        <v>I'm afraid...</v>
+        <v>I'm afraid I can't help you.</v>
       </c>
       <c r="B23" t="str">
-        <v>유감스럽게도 ~인 것 같아.</v>
+        <v>유감스럽지만 널 도와줄 수 없을 것 같아.</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>You'd better...</v>
+        <v>You'd better see a doctor.</v>
       </c>
       <c r="B24" t="str">
-        <v>~하는 게 좋을 거야. (충고/경고)</v>
+        <v>병원에 가보는 게 좋을 거야.</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v>It's hard to...</v>
+        <v>It's hard to believe.</v>
       </c>
       <c r="B25" t="str">
-        <v>~하기 어려워.</v>
+        <v>믿기 힘들어.</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>Is it okay to...?</v>
+        <v>Is it okay to use this phone?</v>
       </c>
       <c r="B26" t="str">
-        <v>~해도 괜찮아?</v>
+        <v>이 전화기 써도 괜찮아?</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Thank you for...</v>
+        <v>Thank you for inviting me.</v>
       </c>
       <c r="B27" t="str">
-        <v>~해줘서 고마워.</v>
+        <v>초대해줘서 고마워.</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>I'm thinking of...</v>
+        <v>I'm thinking of moving to Seoul.</v>
       </c>
       <c r="B28" t="str">
-        <v>~할까 생각 중이야.</v>
+        <v>서울로 이사 갈까 생각 중이야.</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v>What makes you...?</v>
+        <v>What makes you think so?</v>
       </c>
       <c r="B29" t="str">
-        <v>왜 ~하게 된 거야? (이유)</v>
+        <v>왜 그렇게 생각하는 거야?</v>
       </c>
     </row>
     <row r="30">

</xml_diff>